<commit_message>
Changes to MDG4 charts and underlying data files
</commit_message>
<xml_diff>
--- a/data/Data Verification.xlsx
+++ b/data/Data Verification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data Verification" sheetId="1" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>2004, 2009, 2010</t>
   </si>
   <si>
-    <t>Research Paper</t>
-  </si>
-  <si>
     <t>Data Provided by UNKT?</t>
   </si>
   <si>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>Land Usage by Municipality</t>
+  </si>
+  <si>
+    <t>Report on Perinatal Situation in Kosovo</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -457,7 +457,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,7 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -501,10 +500,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="21"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -515,6 +513,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
@@ -529,7 +528,6 @@
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -540,7 +538,6 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -947,7 +944,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -962,7 +959,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
@@ -980,16 +977,16 @@
         <v>43</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1285,8 +1282,8 @@
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>53</v>
+      <c r="D15" t="s">
+        <v>69</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>45</v>
@@ -1301,7 +1298,7 @@
         <v>45</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1312,22 +1309,22 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:9">
@@ -1338,22 +1335,22 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:9">
@@ -1364,7 +1361,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>45</v>
@@ -1384,13 +1381,13 @@
     </row>
     <row r="19" spans="2:9">
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
         <v>64</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>65</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>45</v>
@@ -1416,7 +1413,7 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>45</v>
@@ -1468,7 +1465,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>45</v>
@@ -1488,13 +1485,13 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>45</v>
@@ -1520,10 +1517,10 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>47</v>
@@ -1539,14 +1536,11 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Added Vaccinations chart and modified several existing charts
</commit_message>
<xml_diff>
--- a/data/Data Verification.xlsx
+++ b/data/Data Verification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data Verification" sheetId="1" r:id="rId1"/>
@@ -24,30 +24,6 @@
     <author>Brett Romero</author>
   </authors>
   <commentList>
-    <comment ref="D16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Brett Romero:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Financially supported by UNFPA and UNICEF</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="D17" authorId="0">
       <text>
         <r>
@@ -72,7 +48,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brett Romero:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Financially supported by UNFPA and UNICEF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0">
+    <comment ref="D24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="71">
   <si>
     <t>Data Verification</t>
   </si>
@@ -157,9 +157,6 @@
     <t>1_1</t>
   </si>
   <si>
-    <t>Tab</t>
-  </si>
-  <si>
     <t>Poverty Headcount Ratio at National Poverty Lines</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>4_2</t>
   </si>
   <si>
-    <t>Neonatal Mortality Rate</t>
-  </si>
-  <si>
     <t>5_1</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
     <t>2010, 2011</t>
   </si>
   <si>
-    <t>2004, 2009, 2010</t>
-  </si>
-  <si>
     <t>Data Provided by UNKT?</t>
   </si>
   <si>
@@ -359,6 +350,18 @@
   </si>
   <si>
     <t>Report on Perinatal Situation in Kosovo</t>
+  </si>
+  <si>
+    <t>Early Neonatal Mortality Rate</t>
+  </si>
+  <si>
+    <t>Stillbirth Rate</t>
+  </si>
+  <si>
+    <t>4_3</t>
+  </si>
+  <si>
+    <t>Indicator</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -471,6 +474,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
@@ -502,7 +521,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -528,6 +547,14 @@
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -538,6 +565,14 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -603,10 +638,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:I24" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B3:I24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:I25" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="8">
-    <tableColumn id="1" name="Tab"/>
+    <tableColumn id="1" name="Indicator"/>
     <tableColumn id="2" name="Title" dataDxfId="5"/>
     <tableColumn id="3" name="Source"/>
     <tableColumn id="4" name="Extrapolation Used?" dataDxfId="4"/>
@@ -941,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -965,28 +999,28 @@
     </row>
     <row r="3" spans="1:9" ht="30">
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="F3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -994,545 +1028,571 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="G7" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>45</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>